<commit_message>
Add PIX on employees model
</commit_message>
<xml_diff>
--- a/worksheets/employees.xlsx
+++ b/worksheets/employees.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t xml:space="preserve">nome</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t xml:space="preserve">salario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pix</t>
   </si>
   <si>
     <t xml:space="preserve">data_admissao</t>
@@ -251,32 +254,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -353,210 +360,214 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ3"/>
+  <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AB1" activeCellId="0" sqref="AB1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="21.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="28" style="0" width="15.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="18.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1004" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="1" width="21.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="29" style="1" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1005" style="1" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AC1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="ALP1" s="0"/>
-      <c r="ALQ1" s="0"/>
-      <c r="ALR1" s="0"/>
-      <c r="ALS1" s="0"/>
-      <c r="ALT1" s="0"/>
-      <c r="ALU1" s="0"/>
-      <c r="ALV1" s="0"/>
-      <c r="ALW1" s="0"/>
-      <c r="ALX1" s="0"/>
-      <c r="ALY1" s="0"/>
-      <c r="ALZ1" s="0"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="AE1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="ALQ1" s="1"/>
+      <c r="ALR1" s="1"/>
+      <c r="ALS1" s="1"/>
+      <c r="ALT1" s="1"/>
+      <c r="ALU1" s="1"/>
+      <c r="ALV1" s="1"/>
+      <c r="ALW1" s="1"/>
+      <c r="ALX1" s="1"/>
+      <c r="ALY1" s="1"/>
+      <c r="ALZ1" s="1"/>
+      <c r="AMA1" s="1"/>
+      <c r="AMB1" s="1"/>
+      <c r="AMC1" s="1"/>
+      <c r="AMD1" s="1"/>
+      <c r="AME1" s="1"/>
+      <c r="AMF1" s="1"/>
+      <c r="AMG1" s="1"/>
+      <c r="AMH1" s="1"/>
+      <c r="AMI1" s="1"/>
+      <c r="AMJ1" s="1"/>
+      <c r="AMK1" s="1"/>
     </row>
-    <row r="2" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" s="7" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AA2" s="7" t="s">
         <v>37</v>
       </c>
+      <c r="AD2" s="7" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="3" s="5" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="5" t="s">
+    <row r="3" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="AA3" s="5" t="s">
+      <c r="F3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AC3" s="5" t="s">
+      <c r="AA3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="ALP3" s="6"/>
-      <c r="ALQ3" s="6"/>
-      <c r="ALR3" s="6"/>
-      <c r="ALS3" s="6"/>
-      <c r="ALT3" s="6"/>
-      <c r="ALU3" s="6"/>
-      <c r="ALV3" s="6"/>
-      <c r="ALW3" s="6"/>
-      <c r="ALX3" s="6"/>
-      <c r="ALY3" s="6"/>
-      <c r="ALZ3" s="6"/>
-      <c r="AMA3" s="6"/>
-      <c r="AMB3" s="6"/>
-      <c r="AMC3" s="6"/>
-      <c r="AMD3" s="6"/>
-      <c r="AME3" s="6"/>
-      <c r="AMF3" s="6"/>
-      <c r="AMG3" s="6"/>
-      <c r="AMH3" s="6"/>
-      <c r="AMI3" s="6"/>
-      <c r="AMJ3" s="6"/>
+      <c r="AD3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="ALQ3" s="7"/>
+      <c r="ALR3" s="7"/>
+      <c r="ALS3" s="7"/>
+      <c r="ALT3" s="7"/>
+      <c r="ALU3" s="7"/>
+      <c r="ALV3" s="7"/>
+      <c r="ALW3" s="7"/>
+      <c r="ALX3" s="7"/>
+      <c r="ALY3" s="7"/>
+      <c r="ALZ3" s="7"/>
+      <c r="AMA3" s="7"/>
+      <c r="AMB3" s="7"/>
+      <c r="AMC3" s="7"/>
+      <c r="AMD3" s="7"/>
+      <c r="AME3" s="7"/>
+      <c r="AMF3" s="7"/>
+      <c r="AMG3" s="7"/>
+      <c r="AMH3" s="7"/>
+      <c r="AMI3" s="7"/>
+      <c r="AMJ3" s="7"/>
+      <c r="AMK3" s="7"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>